<commit_message>
updated profile cf script
</commit_message>
<xml_diff>
--- a/ProfileCF/cf_out.xlsx
+++ b/ProfileCF/cf_out.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,16 +484,46 @@
           <t>scholarly</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>officeHours</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>altPhone</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>altPhoneType</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>contactLinks</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>resume</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>photo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>/content/dam/au/cf/html/profiles/staff/tanya</t>
+          <t>/content/dam/au/cf/profiles-migrated/ab/abreetz</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ProfileCF</t>
+          <t>profileCF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,60 +533,39 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>/conf/au/settings/dam/cfm/models/htmlEmbed</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-test of bio with a &lt;a href="https://www.american.edu"&gt;link&lt;/a&gt; in the bio
-</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-&lt;li&gt;
-&lt;p&gt;
-Test Org
-&lt;br&gt;Test Role&lt;/br&gt;&lt;/p&gt;
-&lt;/li&gt;
-</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">
-&lt;div class="col-md-6 col-sm-6 col-xs-12 no-bs-padding-left"&gt;
-&lt;div&gt;&lt;p&gt;Test content&lt;/p&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="col-md-6 col-sm-6 col-xs-12"&gt;
-&lt;/div&gt;
-</t>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>PhD, Clinical Psychology &lt;p&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>/content/dam/au/cf/html/cas/faculty/dabraham</t>
+          <t>/content/dam/au/cf/profiles-migrated/ad/ad5825a</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ProfileCF</t>
+          <t>profileCF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -566,297 +575,369 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>/conf/au/settings/dam/cfm/models/htmlEmbed</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Bachelor of Music Education, Stetson University, 2023 &lt;p&gt;&lt;/p&gt;</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Director, University Pep Band&lt;br&gt;Instrumental Ensemble Manager</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/ad/adaniels</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/af/afkaplan</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">
-Choral/orchestral conductor and musicologist; specialist in 17th- and 18th-century music. &lt;br/&gt;&lt;br/&gt;As a conductor and scholar, Abraham has often sought out works previously unknown to present-day audiences and has been responsible for numerous world, North American, and regional early-music modern premieres with many performances using materials he has edited from archival manuscript sources. Abraham has conducted performances before two National Meetings of the American Musicological Society, has been broadcast nationally on NPR’s Performance Today, Great Sacred Music, and Sunday Baroque, and has appeared at the John F. Kennedy Center for the Performing Arts, the Music Center at Strathmore, the National Women’s Museum of the Arts, the National Portrait Gallery, the Cosmos Club, and many other venues in the eastern United States. Guest conducting appearances include concerts with the Trinity Wall Street Baroque Orchestra and Trinity Chorus (New York), as conductor of the Massachusetts Northwestern All-State Chorus, and internationally with various university and professional ensembles in Bosnia and Herzegovina, Canada, Colombia, Croatia, Czechia, Germany, Greece, Hungary, Kosovo, Macedonia, Montenegro, Poland, Portugal, Romania, Russia, Slovakia, Spain, and in Egypt where he was Visiting Distinguished Professor of the Arts. &lt;br/&gt;&lt;br/&gt;He has garnered praise for his performances from many noteworthy sources, including Gramophone, the Washington Post, Choral Journal, BBC Magazine, Fanfare, Diapason, BBC Radio 3, American Record Review, and Early Music America. In addition to his work in early music, he is a champion of new composition particularly of American and Canadian choral composers. &lt;br/&gt;&lt;br/&gt;He served as Artistic Director and Conductor of The Bach Sinfonia for twenty-one seasons, appeared on the nationally syndicated PBS series History Detectives, and has prepared choruses for national television broadcast including the Kennedy Center Honors Gala and Christmas in Washington as well as notable conductors including Lenard Slatkin, Michael Tilson Thomas, Leon Botstein and with artists including Ray Charles, Andrea Bocelli, and Kristin Chenoweth. He has presented papers before the American Musicological Society and at national and regional meetings of the American Choral Director Association. &lt;br/&gt;&lt;br/&gt;In addition to his six commercial audio recordings on the Chandos, Dorian and Sonoluminus labels, his recent scholarly work includes: the National Endowment for the Humanities (NEH) funded multidisciplinary immersive audio project “Hearing Bach’s Acoustic” with audio technologist Braxton Boren, interactive-media designer Yana Sakellion, and audio engineer Rogerio Naressi; a critical edition of choral music by Heinrich Biber for Carus Verlag; and co-editing, with Alicia Kopfstein-Penk and Andrew Weaver, the volume Leonard Bernstein and Washington, DC: Works, Politics, and Performance for Eastman Studies in Music (University of Rochester Press). His recent commercial recording, ALTISSIMA, with baroque trumpet virtuoso Josh Cohen, was released in January 2023 on the Chandos label. Published in Choral Journal, editorial work for The Carl Philipp Emanuel Bach Edition (OUP), and Cambridge University Press. Past grant panelist for the Maryland State Arts Council, DC Commission on the Arts, and the Arts and Humanities Council of Montgomery Country (MD). Past President of the MD/DC State Chapter of the American Choral Directors Association. Conducting studies and additional training with Paul Traver, Helmuth Rilling, William Weinert, Frieder Bernius, and David Hoose. Abraham is a sought-after clinician, adjudicator, and festival ensemble conductor.
+Anna Kaplan researches and teaches 20th Century US history and public history. Her focus is memory and the creation and uses of public narratives about race, particularly African American, white, and Indigenous dynamics in the US South. She is working on a manuscript examining how Oxford, MS, communities and the university constructs and employs stories about the University of Mississippi’s desegregation in 1962. She is also researching the erased history of Black women’s contributions to early institutional oral history programs. She has worked on oral history projects for the US Department of State, the National Park Service, the National Endowment for the Humanities, the Smithsonian Institution's Archives of American Art, and more local DC community organizations. She was one of the founders of the DC Oral History Collaborative and continues to develop and lead community workshops for the program. In addition, Anna serves as the President of Oral History in the Mid-Atlantic Region and on the Nominating Committee for the Oral History Association. She is a 2023-2024 HistoryMakers Faculty Innovations in Pedagogy and Teaching Fellow. Her article “Everyday Activism: How Local Black Residents Shaped the University of Mississippi and Oxford in the Mid-20th Century” is forthcoming in 2024 in the journal Study the South.
 </t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>BM Music, University of Massachusetts&lt;br&gt;MM Historical Musicology &amp;amp; Conducting, University of Maryland&lt;br/&gt; &lt;p&gt;&lt;/p&gt;&lt;/br&gt;</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>&lt;a href="https://www.american.edu/cas/performing-arts/music/"&gt;Professor of Music&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.american.edu/cas/performing-arts/index.cfm"&gt;Director of Choral Activities, spring 1999-present&lt;/a&gt;&lt;br&gt;&lt;a href="https://www.american.edu/cas/performing-arts/music/"&gt;Chair of Department of Performing Arts, 2020-present; 2009-2011; 2014-2017 &amp;amp; Director of Music, 2000-2006&lt;/a&gt;</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>PhD, History with Public History concentration, American University&lt;br&gt;MA, Oral History, Columbia University&lt;br&gt;MA, Anthropology, Columbia University&lt;br/&gt;BA, Anthropology, Folklore and Creative Writing minors, University of North Carolina at Chapel Hill &lt;p&gt;&lt;/p&gt;&lt;/br&gt;&lt;/br&gt;</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/migrated-profile-resumes/uploads/docs/AFKaplanCV11.2023.pdf</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/migrated-profile-images/uploads/profiles/original/Kaplan_Headshot2_300x300_1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/ag/agretarsson</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/aj/ajorgo</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/ak/akeshta</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
         <is>
           <t xml:space="preserve">
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="http://acda.org/"&gt;American Choral Directors Association&lt;/a&gt;
-&lt;br/&gt;State President (Maryland/District of Columbia), 2009-2011; Interest Session Chair, Eastern Division, 2008-2010&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="https://www.msac.org/"&gt;Maryland State Arts Council&lt;/a&gt;
-&lt;br/&gt;Panelist/Reviewer, 2004-2006&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="http://www.ams-net.org/"&gt;American Musicological Society&lt;/a&gt;
-&lt;br/&gt;Secretary-Treasurer, Capitol Chapter, 2000-2003&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-The Bach Sinfonia &amp;amp; Sinfonia Voci
-&lt;br/&gt;Music &amp;amp; Artistic Director, 1995-2016&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="https://www.kennedy-center.org/wno/"&gt;Washington National Opera Institute for Young Singers&lt;/a&gt;
-&lt;br/&gt;Chorus Master, 2009-2021&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="https://acda.org/"&gt;American Choral Directors Association&lt;/a&gt;
-&lt;br/&gt;Chair, Research &amp;amp; Publications: Monographs Sub-committee (National), 2016-present&lt;/p&gt;
-&lt;/li&gt;
-&lt;li&gt;
-&lt;p&gt;
-&lt;a href="https://dcarts.dc.gov/"&gt;DC Commission on the Arts and Humanities&lt;/a&gt;
-&lt;br/&gt;Grant Panelist, 2021-present&lt;/p&gt;
-&lt;/li&gt;
+Research Biogeochemist and Professional GIS analyst (GISP). Expertise in Wetland Ecosystem Ecology, Biogeochemical Cycling, and Coastal Ecosystems.
 </t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ph.D., Department of Environmental Science and Technology, College of Agriculture and Natural Resources, University of Maryland, College Park, Maryland, USA. &lt;br&gt;&lt;br&gt;M.S., Department of Botany and Microbiology, College of Science, Tanta University, Tanta, Egypt.&lt;br/&gt;&lt;br/&gt;B.S., Department of Botany and Microbiology, College of Science, Tanta University, Tanta, Egypt &lt;p&gt;&lt;/p&gt;&lt;/br&gt;&lt;/br&gt;</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/migrated-profile-images/uploads/profiles/original/AmrKeshta_AU.JPG</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/ak/akowalevicz</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/am/amannur</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
         <is>
           <t xml:space="preserve">
-&lt;div class="col-md-6 col-sm-6 col-xs-12 no-bs-padding-left"&gt;
-&lt;div&gt;&lt;h3&gt;Research Interests&lt;/h3&gt;&lt;p&gt;Performance and research in baroque and classical period music (17th and 18th centuries); issues in performance practice; the music of Bach and Handel, choral music research and pedagogy.&lt;/p&gt;&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Honors, Awards, and Fellowships&lt;/h3&gt;&lt;h4&gt;Professional Honors, Awards &amp;amp; Distinctions&lt;/h4&gt;
-&lt;ul&gt;
-&lt;li&gt;Second Prize, The American Prize in Composition (Major Work): Arnold Saltzman: &lt;i&gt;A Choral Symphony: Halevi, &lt;/i&gt;2025 (role: choral preparation)&lt;/li&gt;
-&lt;li&gt;&lt;i&gt;Dean’s Award for Exceptional Innovation&lt;/i&gt;, College of Arts and Sciences. Faculty of the Department of Performing Arts &amp;amp; Staff of the Katzen Arts Center and Greenberg Theatre, 2021&lt;/li&gt;
-&lt;li&gt;American University Alumni Engagement Award, 2018&lt;/li&gt;
-&lt;li&gt;Washington Area Music Association Awards (WAMMIES), multiple nominations:&lt;/li&gt;
-&lt;li&gt;Best Classical Conductor/Director; 2014, 2013, 2012, 2011&lt;/li&gt;
-&lt;li&gt;Best Classical Chamber Ensemble (Bach Sinfonia), 2014, 2013, 2012, 2011&lt;/li&gt;
-&lt;li&gt;Best Classical Recording: &lt;i&gt;Zelenka: The Capriccios&lt;/i&gt;, 2013, &lt;i&gt;J. S. Bach: Motets,&lt;/i&gt; 2012 &amp;amp; &lt;i&gt;The Art of Vivaldi’s Lute&lt;/i&gt;, 2012&lt;/li&gt;
-&lt;li&gt;Second Prize, The American Prize, Bach Sinfonia Voci, Choral Performance (Professional Ensemble), 2011&lt;/li&gt;
-&lt;li&gt;Appointed Member, Maryland States Arts Council, 2003–2006&lt;/li&gt;
-&lt;li&gt;Distinguished Visiting Professor in the Performing and Visual Arts, American University Cairo (Egypt), spring 2005&lt;/li&gt;
-&lt;li&gt;(American University Cairo is not affiliated with American University, Washington, D.C.)   &lt;/li&gt;
-&lt;li&gt;Daniel M. Pomeroy Prize, American Handel Society (Performance &amp;amp; Scholarship in Eighteenth–Century Music), 1998&lt;/li&gt;
-&lt;li&gt;Irving Lowens Award, American Musicological Society, Capital Chapter, Excellence in Musicological Research, 1996&lt;/li&gt;
-&lt;/ul&gt;
-&lt;h4&gt;Special Recognition of Recordings &amp;amp; Performances&lt;/h4&gt;
-&lt;ul&gt;
-&lt;li&gt;No. 1 on Amazon (USA) Early Music New Releases for 5 weeks (January 27-March 3, 2023), &lt;i&gt;Altissima:&lt;/i&gt;&lt;i&gt; The High Register Baroque Trumpet&lt;/i&gt;&lt;/li&gt;
-&lt;li&gt;Top 30 on UK Official Charts for 6 weeks (Record Sales), reached No. 7 — Classical for 4 weeks (January 20-March 3, 2023), &lt;i&gt;Altissima:&lt;/i&gt;&lt;i&gt; The High Register Baroque Trumpet&lt;/i&gt;. Ensemble Sprezzatura.&lt;i&gt; &lt;/i&gt;Josh Cohen, baroque trumpet; Daniel Abraham, director/conductor and project producer. Chandos Records CHAN 0828 (UK), January 2023&lt;/li&gt;
-&lt;li&gt;NPR’s Sunday Baroque, selection of &lt;i&gt;Zelenka: The Capriccios &lt;/i&gt;as one of 2013’s Top Classical CDs, 2013&lt;/li&gt;
-&lt;li&gt;Audiophile Audition: Multi-Channel Disc of the Month (&lt;i&gt;Zelenka: The Capriccios&lt;/i&gt;), October 2013&lt;/li&gt;
-&lt;li&gt;iTunes Classical: “New and Noteworthy” &lt;i&gt;Zelenka: The Capriccios, &lt;/i&gt;November 2012&lt;i&gt;&lt;/i&gt;&lt;/li&gt;
-&lt;li&gt;Naxos’ Critical Choice Selection, &lt;i&gt;The Bach Motets,&lt;/i&gt; July 2011&lt;/li&gt;
-&lt;li&gt;Classical WETA–FM&lt;i&gt; &lt;/i&gt;90.9, &lt;i&gt;Art of Vivaldi’s Lute&lt;/i&gt; (vocal highlight of the week), June 27–July 3, 2011&lt;/li&gt;
-&lt;li&gt;Naxos’ Critical Choice Selection, The Bach Motets, April 2011&lt;/li&gt;
-&lt;li&gt;Classical WETA–FM, VivaLaVoce: &lt;i&gt;J. S. Bach: Motets&lt;/i&gt; (vocal highlight of the week), March 7–13, 2011&lt;/li&gt;
-&lt;li&gt;“Arts &amp;amp; Style: 2010 Fall Arts Preview”, Bach Sinfonia’s &lt;i&gt;’Til Death Do Us Part &lt;/i&gt;(October 2010)&lt;i&gt; &lt;/i&gt;selected as one of three fall Classical Critic’s Choices, &lt;i&gt;The Washington Post, &lt;/i&gt;September 12, 2010, E15&lt;/li&gt;
-&lt;li&gt;Classical WETA–FM, VivaLaVoce: &lt;i&gt;Passion &amp;amp; Lament &lt;/i&gt;(vocal highlight of the week), May 31–June 31, 2010&lt;/li&gt;
-&lt;li&gt;“Best of Washington’s Performances, 2006” (Performances of Purcell’s &lt;i&gt;Dido &amp;amp; Aeneas&lt;/i&gt; by Bach Sinfonia and Chantry, October 2006 selected as second in critic’s list of top-ten performances in Washington D.C.); Andrew Lindemann Malone, &lt;i&gt;The Washington Post&lt;/i&gt; and DMVClassical.com, December 2006&lt;/li&gt;
-&lt;li&gt;“Newly Discovered Musical Composition by Handel: &lt;i&gt;Gloria in excelsis Deo&lt;/i&gt;—Noteworthy Performances”, 2006&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Professional Presentations&lt;/h3&gt;&lt;ul&gt;
-&lt;li&gt;Workshop panelist/discussant, “The Educational Value of Sport.” American University, October 2025&lt;/li&gt;
-&lt;li&gt;Knight Commission on Intercollegiate Athletics, panelist, “The Art of Sport: Learning, Performance, and Pedagogy.” &lt;i&gt;Symposium on the Educational Value of Sport, &lt;/i&gt;October 2025&lt;/li&gt;
-&lt;li&gt;“What is a Twenty-First Century Music Conservatory?” University of Denver, February 2025&lt;i&gt;&lt;/i&gt;&lt;/li&gt;
-&lt;li&gt;“Be Not Afraid: Strategies for Exploring Works with Non-Traditional Notation.” Washington DC Music Education Association.&lt;i&gt; &lt;/i&gt;American University Chamber Singers/Daniel Abraham, director, January 2024&lt;/li&gt;
-&lt;li&gt;“Acoustic Simulation of Bach’s Performing Forces in the Thomaskirche.” Conference Paper and Proceedings, with co-author Braxton Boren. European Acoustics Association. Paris, France, September 2019&lt;/li&gt;
-&lt;li&gt;“The Multi-Disciplinary Conservatory: Preparing Career Readiness and Innovators of the Future.” Address, Western Australia Academy of the Performing Arts, Perth, Australia. November 2018&lt;/li&gt;
-&lt;li&gt;“A Vision for the 21&lt;sup&gt;st&lt;/sup&gt; Century Conservatory”, Keynote Speaker, University of the Pacific, Stockton, California. Dec. 2016&lt;/li&gt;
-&lt;li&gt;“Creating a (non-Profit) Ensemble.” Panelist,&lt;i&gt; Conductor’s Guild National Conference&lt;/i&gt;, June 2014&lt;/li&gt;
-&lt;li&gt;“The Search for An American Style: Composer’s Panel.” Convener &amp;amp; Moderator (Libby Larsen, Gwyneth Walker, David Conte); &lt;i&gt;National Symposium for American Choral Music&lt;/i&gt;, Library of Congress &amp;amp; American Choral Directors Association, June 2012&lt;/li&gt;
-&lt;li&gt;“The Search for An American Style: Scholar–Conductor’s Panel.” Convener &amp;amp; Moderator (David DeVenney, James John, Philip Brunelle); &lt;i&gt;National Symposium for American Choral Music&lt;/i&gt;, Library of Congress &amp;amp; American Choral Directors Association, June 2012&lt;/li&gt;
-&lt;li&gt;“Performing Early Music: Working as an Informed Performer.” Lecture, Boyer School of Music, Temple University, Philadelphia, Pennsylvania, November 2011&lt;/li&gt;
-&lt;li&gt;“Suoni Belli: The Allure of Italian Baroque Instrumental Music.” Lecture, National Humanities Month, Montgomery College, Takoma Park, Maryland, October 2011&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;Preparing the Parts: Efficient Marking for Choral-Instrumental Performance. &lt;/em&gt;Conference Interest Session. American Choral Directors Association, Eastern Division Conference, Philadelphia, Pennsylvania, February 13, 2010&lt;/li&gt;
-&lt;li&gt;&lt;!--EndFragment--&gt;&lt;em&gt;New Editions of Old Music. &lt;/em&gt;Conference Session for the College and University Conductor’s Repertoire Forum. American Choral Directors Association, Eastern Division Conference, Hartford, Connecticut, February 19, 2008&lt;/li&gt;
-&lt;li&gt;Collegiate Honor Choir Chair, 2008 Eastern Division Conference, American Choral Directors Association, Hartford, Connecticut, February 2008  &lt;/li&gt;
-&lt;li&gt;Collegiate Honor Choir Chair, 2006 Eastern Division Conference, American Choral Directors Association, New York, New York, February 2006&lt;/li&gt;
-&lt;li&gt;Appearance on premiere season of "The History Detectives," PBS Television, 2003&lt;/li&gt;
-&lt;li&gt;Frequent clinician, adjudicator, and festival conductor throughout the eastern United States and Canada&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Recordings&lt;/h3&gt;&lt;ul&gt;
-&lt;li&gt;&lt;i&gt;Altissima:&lt;/i&gt;&lt;i&gt; The High Register Baroque&lt;/i&gt;. Ensemble Sprezzatura.&lt;i&gt; &lt;/i&gt;Josh Cohen, baroque trumpet; Daniel Abraham, director/conductor and project producer. Chandos Records CHAN 0828 (UK), January 2023.&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;Zelenka: The Capriccios. &lt;/em&gt;The Bach Sinfonia; R.J. Kelley &amp;amp; Alexandra Cook, natural horns. Sono Luminus Records, November 2012&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;The Art of Vivaldi's Lute. &lt;/em&gt;The Bach Sinfonia; Ronn McFarlane, lute; William Bauer, Viola d'amore; Jennifer Ellis, soprano. Sono Luminus Records, May 2011&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;J. S. Bach: The Motets&lt;/em&gt;. The Bach Sinfonia and Sinfonia Voci; Dorian Records, October 2010&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;The Forgotten Baroque: Masterworks of the Seventeenth Century.&lt;/em&gt; Biber: Stabat Mater [modern premiere recording], Rossi: psalms &amp;amp; Carissimi: Historia di Jephte. The Bach Sinfonia and Sinfonia Voci; Dorian Records, May 2009&lt;/li&gt;
-&lt;li&gt;&lt;em&gt;George Frideric Handel: Alexander’s Feast or The Power of Music, HWV 75 and Johann Sebastian Bach: Alles mit Gott und nichts ohn’ ihn, BWV 1127.&lt;/em&gt; The Bach Sinfonia and Handel Choir of Baltimore. Dorian Records: DSL-20604, December 2006&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;strong&gt;Selected Reviews of Recordings&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;“&lt;i&gt;Altissima: Works For High Baroque Trumpet &lt;/i&gt;Josh Cohen (trumpet); Daniel Abraham (conductor); Ensemble Sprezzatura Chaconne 0828” &lt;i&gt;Fanfare, &lt;/i&gt;Vol 47/1&lt;i&gt;, &lt;/i&gt;September/October 2023 by Michael De Sapio.&lt;/li&gt;
-&lt;li&gt;“Zesty Music for High Baroque Trumpet” &lt;i&gt;Early Music America, &lt;/i&gt;September 2023 by Aaron Keebaugh. &lt;a href="https://www.earlymusicamerica.org/web-articles/zesty-music-for-high-baroque-trumpet/"&gt;https://www.earlymusicamerica.org/web-articles/zesty-music-for-high-baroque-trumpet/&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“&lt;i&gt;Altissima: Works for High Baroque Trumpet &lt;/i&gt;• Josh Cohen (tpt); Daniel Abraham, conductor; Ensemble Sprezzatura • Chaconne 0828” &lt;i&gt;Fanfare, &lt;/i&gt;Vol 46/6&lt;i&gt;, &lt;/i&gt;July/August 2023 by James A. Altena&lt;/li&gt;
-&lt;li&gt;“Altissima; Works for High Baroque Trumpet” &lt;i&gt;Classical Explorer, &lt;/i&gt;July 29, 2023 by Colin Clarke. &lt;a href="https://www.classicalexplorer.com/altissima-works-for-high-baroque-trumpet/"&gt;https://www.classicalexplorer.com/altissima-works-for-high-baroque-trumpet&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Altissima: Josh Cohen, Works for High Baroque Trumpet” &lt;i&gt;Historic Brass Society, &lt;/i&gt;June 17, 2023 by Jason Duvol. &lt;a href="https://www.historicbrass.org/features/reviews/recording-reviews/josh-cohen-altissima-works-for-high-baroque-trumpet"&gt;https://www.historicbrass.org/features/reviews/recording-reviews/josh-cohen-altissima-works-for-high-baroque-trumpet&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Copieux récital de trompette baroque dans la sphère germanique” (“A hearty baroque trumpet recital in the Germanic sphere”) C&lt;i&gt;rescendo &lt;/i&gt;(Belgium). March 17, 2023 by Christophe Steyne. &lt;a href="https://www.crescendo-magazine.be/copieux-recital-de-trompette-baroque-dans-la-sphere-germanique/?fbclid=IwAR2pgAJjffBqdpXPDDMuibqJ-Cwby6Vzj7yjoXkxh-zRBitoGjed0Dc8BEg"&gt;https://www.crescendo-magazine.be/copieux-recital-de-trompette-baroque-dans-la-sphere-germanique/?fbclid=IwAR2pgAJjffBqdpXPDDMuibqJ-Cwby6Vzj7yjoXkxh-zRBitoGjed0Dc8BEg&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Altissima: Works for High Baroque Trumpet (Josh Cohen)/Chandos” &lt;i&gt;Gramophone. &lt;/i&gt;March&lt;i&gt; &lt;/i&gt;2023 by Jonathan Freeman-Attwood.&lt;/li&gt;
-&lt;li&gt;“Altissima: Works for High Baroque Trumpet Review.”&lt;i&gt; AllMusic.&lt;/i&gt; February 22, 2023 by James Manheim. &lt;a href="https://www.allmusic.com/album/altissima-works-for-high-baroque-trumpet-mw0003877874"&gt;https://www.allmusic.com/album/altissima-works-for-high-baroque-trumpet-mw0003877874&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Altissima — Works for High Baroque Trumpet” &lt;i&gt;BBC Magazine &lt;/i&gt;(UK). February 21, 2023 by Nicholas Anderson. &lt;a href="https://www.classical-music.com/reviews/concerto/altissima-works-for-high-baroque-trumpet/"&gt;https://www.classical-music.com/reviews/concerto/altissima-works-for-high-baroque-trumpet/&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Album van de Week: Baroktrompettist Josh Cohen speelt de sterren van de hemel op zijn nieuwe album &lt;i&gt;Altissima.&lt;/i&gt; Een cd vol Barokke trompetglorie.” (“Album of the Week: Baroque trumpeter Josh Cohen plays the stars from heaven on his new album Altissima. A CD full of Baroque trumpet glory.”) &lt;i&gt;NPO Radio 4&lt;/i&gt; (NPO Klassiek, Netherlands), February 5, 2023 by Sander Zwiep. &lt;a href="https://www.nporadio4.nl/klassiek/album-van-de-week/46d331da-af7e-4626-9c59-4add132e1424/altissima-works-for-high-baroque-trumpet"&gt;https://www.nporadio4.nl/klassiek/album-van-de-week/46d331da-af7e-4626-9c59-4add132e1424/altissima-works-for-high-baroque-trumpet&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Altissima: Work for High Baroque Trumpet.” &lt;i&gt;BBC 3: Record Review, &lt;/i&gt;January 28, 2023 by Laurence Cummings.&lt;/li&gt;
-&lt;li&gt;“Altissima: musica per tromba naturale barocca - Josh Cohen/Ensemble Sprezzatura.” &lt;i&gt;Nikonland &lt;/i&gt;(Italy)&lt;i&gt;, &lt;/i&gt;January 24, 2023.  &lt;a href="https://www.nikonland.it/index.php?/blogs/entry/1495-altissima-musica-per-tromba-naturale-barocca-josh-cohenensemble-sprezzatura/"&gt;https://www.nikonland.it/index.php?/blogs/entry/1495-altissima-musica-per-tromba-naturale-barocca-josh-cohenensemble-sprezzatura/&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Classical Music: Altissima Works For High Baroque Trumpet.” &lt;i&gt;Cumbria Times &lt;/i&gt;(UK)&lt;i&gt;, &lt;/i&gt;January 21, 2023 by Andrew Palmer. &lt;a href="https://cumbriatimes.co.uk/article/Classical-Music-Altissima--Works-For-High-Baroque-Trumpet"&gt;https://cumbriatimes.co.uk/article/Classical-Music-Altissima--Works-For-High-Baroque-Trumpet&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;“Jan Dismas Zelenka: The Capriccios (Five)—The Bach Sinfonia/Daniel Abraham—Sono Luninus Pure Audio Blu-ray+CD.” &lt;i&gt;Audiophile Audition,&lt;/i&gt; October 24, 2013; critical review by John Sunier. [Selection as “Multichannel Disc of the Month”]&lt;/li&gt;
-&lt;li&gt;“Zelenka: The Capriccios [The Bach Sinfonia]; Blu-ray Audio Review.” &lt;i&gt;Blu-RayDefinition.com,&lt;/i&gt; June 23, 2013; critical review by Lawrence D. Devoe&lt;/li&gt;
-&lt;/ul&gt;
-&lt;ul&gt;
-&lt;li&gt; &lt;/li&gt;
-&lt;li&gt;Nelson, David. “Zelenka: A Survey of His Music Now or Very Recently Available on CD.” 58 pages. &lt;em&gt;Czech Music, the Journal of the Dvořák Society&lt;/em&gt; (2012; updated on-line: May 2013); “Capriccios ZWV 182/5,190,” pp. 52-53. &lt;/li&gt;
-&lt;li&gt;“Johann Sebastian Bach: Motets.” &lt;em&gt;Choral Journal&lt;/em&gt; (February 2013), 75-6; critical review by Garrett Saake.&lt;/li&gt;
-&lt;li&gt;"Vivaldi: Lute Pieces." &lt;em&gt;American Record Guide &lt;/em&gt;(November 2011), 189; critical review by Peter Loewen.&lt;/li&gt;
-&lt;li&gt;"Ronn McFarlane's lute is ever present in this varied and pleasurable programme." &lt;em&gt;Gramophone&lt;/em&gt; (October 2011); critical review by Donald Rosenberg.&lt;/li&gt;
-&lt;li&gt;"Johann Sebastian Bach: Motets."&lt;em&gt; Early Music America&lt;/em&gt; 17 (Summer 2011), 21-2; critical review by Karen Cook.&lt;/li&gt;
-&lt;li&gt;"Vivaldi by Ronn McFarlane and Daniel Abraham." &lt;em&gt;WETA&lt;/em&gt;, June 2011; critical review. "Daniel Abraham: Bach's 7 Motets on Dorian." &lt;em&gt;Fanfare&lt;/em&gt; 34:4 (March/April 2011); critical review by George Chien.&lt;/li&gt;
-&lt;li&gt;"Classical: Bach Motets Performed by Bach Sinfonia." &lt;em&gt;The Buffalo News,&lt;/em&gt; March 4, 2011; critical review by Mary Kunz Goldman.&lt;/li&gt;
-&lt;li&gt;"Bach: Motets." &lt;em&gt;American Record Guide&lt;/em&gt; (January 2011), 82-3; critical review by Lindsay Koob.&lt;/li&gt;
-&lt;li&gt;"J.S. Bach: Motets (Bach Sinfonia, Abraham)." &lt;em&gt;Audio Video of Atlanta&lt;/em&gt;, December 2010; critical review by Phil Muse.&lt;/li&gt;
-&lt;li&gt;"Classical CD Reviews: Passion and Lament." &lt;em&gt;Audiophile Audition&lt;/em&gt; (July 1, 2010), critical review by Steven Ritter.&lt;/li&gt;
-&lt;li&gt;"Winning affections: Paul Riley is moved by Daniel Abraham collection of Baroque choral works." &lt;em&gt;BBC Magazine&lt;/em&gt; (June 2010), U.S. Reviews, 97; critical review by Paul Riley.&lt;/li&gt;
-&lt;li&gt;"Recording Reviews: Passion and Lament: Choral Masterworks of the 17th Century."&lt;em&gt; Early Music America&lt;/em&gt; (summer 2010), 50-1; critical review by Karen Cook.&lt;/li&gt;
-&lt;li&gt;"CD Review: Building a Library: Carissimi's Jephte." &lt;em&gt;BBC Radio 3&lt;/em&gt;; broadcast: Saturday, May 15, 2010 and podcast available (time: 26:44-1:17:18); critical review by David Vickers.&lt;/li&gt;
-&lt;li&gt;Recording Reviews: G. F. Handel: Alexander's Feast, or The Power of Music, HWV 75; Johann Sebastian Bach: Alles mit Gott und nichts ohn ihn, BVW 1127; Daniel Abraham, conductor; Dorian Recordings. &lt;em&gt;Choral Journal, &lt;/em&gt;September 2007, critical review by C. Leonard Raybon, pp. 71-73.&lt;/li&gt;
-&lt;li&gt;Recording Review of G. F. Handel: Alexander's Feast / J. S. Bach: Alles mit Gott und nichts ohn ihn, BVW 1127 (Dorian DSL-20604) in &lt;em&gt;Early Music America,&lt;/em&gt; September 2007, critical review by Denise Gallo&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-&lt;div class="col-md-6 col-sm-6 col-xs-12"&gt;
-&lt;div&gt;&lt;h3&gt;Selected Publications&lt;/h3&gt;&lt;ul&gt;
-&lt;li&gt;&lt;em&gt;Renaissance and Baroque Performance Practice: Invaluable Resources for the Choral Conductor&lt;/em&gt; (with James John, co-author). &lt;em&gt;Research Memorandum Series, No. 200. &lt;/em&gt;Chorus America: Philadelphia, 2011.&lt;/li&gt;
-&lt;li&gt;"Vivaldi's Works for Lute and Ensemble” for Indianapolis Early Music Festival, Summer, 2011 [program annotation]&lt;/li&gt;
-&lt;li&gt;“Mozart’s Requiem: History and its Conclusions” for Handel Choir of Baltimore, May 2011 [program annotation]&lt;/li&gt;
-&lt;li&gt;“Vivaldi and the Concerto” for The Art of Vivaldi’s Lute, Ronn MacFarlane and The Bach Sinfonia. Sono Luninus, October 2011 [CD recording annotation]&lt;/li&gt;
-&lt;li&gt;“New Bach Performances: Historically Informed?” &lt;em&gt;Choral Journal,&lt;/em&gt; April 2008   &lt;/li&gt;
-&lt;li&gt;"The London Pleasure Gardens and their Musical Entertainments” for Songs of the London Pleasure Gardens, Brandywine Baroque for Plectra Records, PL20601: December 2006 [CD recording annotation]   &lt;/li&gt;
-&lt;li&gt;“&lt;em&gt;Alles mit Gott und nichts ohn’ ihn&lt;/em&gt;: A newly discovered aria by Johann Sebastian Bach” for Dorian Records: DSL-20604, December 2006 [CD recording annotation]&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Grants and Sponsored Research&lt;/h3&gt;&lt;ul&gt;
-&lt;li&gt;National Endowment for the Humanities (NEH), Digital Humanities Advancement Grant, &lt;i&gt;Hearing&lt;/i&gt; &lt;i&gt;Bach’s Acoustics, &lt;/i&gt;Phase 1:&lt;i&gt; &lt;/i&gt;2018-20 ($50,000; 11.6% acceptance rate) [collaborator: Braxton Boren, music technologist and Yana Sakellion, interactive media designer]&lt;/li&gt;
-&lt;li&gt;&lt;i&gt;Altissima. &lt;/i&gt;Recording project: private, small grant, and crowd sourced funding, 2018-2020 ($26,400)&lt;/li&gt;
-&lt;li&gt;Maryland State Arts Council: Arts Organization Support for mid-size Organizations, Arts in the Community Grants, and General Operating Support (The Bach Sinfonia): 2001, 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016 [$3,100-7,500]&lt;/li&gt;
-&lt;li&gt;Arts and Humanities Council of Montgomery County (Maryland): Grant for Artistic Organizations &amp;amp; Administrative Support (The Bach Sinfonia): 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009, 2010, 2011, 2012, 2013, 2014, 2015, 2016 [$25,000-38,000]&lt;/li&gt;
-&lt;li&gt;U.S. Department of State, Embassy of Moscow, Travel Assistance Grant, 2013 ($10,000)&lt;/li&gt;
-&lt;li&gt;Grant from Ernst and Young, LLP: General Arts Support (The Bach Sinfonia): 2002, 2003, 2004, 2005, 2006, 2007, 2008, 2009 [$3,000-7,500]&lt;/li&gt;
-&lt;li&gt;The Dimick Foundation, Artistic Support (The Bach Sinfinia): 2003, 2004, 2005, 2006&lt;/li&gt;
-&lt;li&gt;Lockheed-Martin, Arts and Technology Grant (The Bach Sinfonia): 2004&lt;/li&gt;
-&lt;li&gt;University of Maryland, Project Support Grant, 2002&lt;/li&gt;
-&lt;li&gt;Prince George’s County Arts Council, 2000&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Media Appearances&lt;/h3&gt;&lt;p&gt;&lt;strong&gt;Selected Feature Articles &amp;amp; Media Interviews&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;“‘Defiant Requiem,’ helping keep the Holocaust in public memory for 20 years.”  &lt;i&gt;The Hub: League of American Orchestras, &lt;/i&gt;April 19, 2022&lt;/li&gt;
-&lt;li&gt;“‘Defiant Requiem’ mines musical hope from horrors of the Holocaust.” &lt;i&gt;The Washington Post, &lt;/i&gt;April 15, 2022 by Mchael Andor Brodeur&lt;/li&gt;
-&lt;li&gt;“What Did Bach Sound Like to Bach? Scholars look to recover the original soundscape of the composer’s work.” &lt;i&gt;Humanities&lt;/i&gt;, 41/2 (Spring 2020) by Paula Wasley&lt;/li&gt;
-&lt;li&gt;“Journeys Medieval and Modern” (Halevi Symphony). &lt;i&gt;Washington Jewish Week &lt;/i&gt;(February 2019) by Lisa Traiger&lt;/li&gt;
-&lt;li&gt;“Early Music is a Capital Idea.” Early Music America 20/1 (Winter 2014): 34-8 by Mark Longaker.   &lt;/li&gt;
-&lt;li&gt;“Chamber music’s timelessness explored.” The Gazette Newspapers (Maryland), February 2, 2013 by Marie Gullard.&lt;/li&gt;
-&lt;li&gt;“Spotlight—The Arts Served Daily: The Bach Sinfonia presents Zelenka.” Metro Weekly, May 2, 2012 by Randy Shulman.&lt;/li&gt;
-&lt;li&gt;“Concert brings Bach to the future at Montgomery College’s Cultural Arts Center; Concert reenacts composer’s job audition to let modern audience decide.” The Gazette Newspapers (Maryland), March 28, 2012 by Cody Calamaio.&lt;/li&gt;
-&lt;li&gt;“Audience Rates 18th Century Performances in Real–Time Voting.” Washington Examiner. March 27, 2012 by Marie Gullard.&lt;/li&gt;
-&lt;li&gt;Vivaldi Goes Digital: Bach Sinfonia put multimedia spin on 'The Four Season.'" &lt;em&gt;The Gazette Newspapers &lt;/em&gt;(Maryland),May 4, 2011 by Jordan Edwards.&lt;/li&gt;
-&lt;li&gt;"Concert brings Bach to the future at Montgomery College's Cultural Arts Center; Concert reenacts composer's job audition to let modern audience decide."&lt;em&gt;The Gazette Newspapers&lt;/em&gt; (Maryland), May 28, 2012 by Cody Calamato&lt;/li&gt;
-&lt;li&gt;&lt;span&gt;"Audience Rates 18th Century Performances in Real–Time Voting." &lt;em&gt;Washington Examiner. &lt;/em&gt;March 27, 2012 By Marie Gullard&lt;/span&gt;&lt;/li&gt;
-&lt;li&gt;"Vivaldi Goes Digital: Bach Sinfonia puts multimedia spin on 'The Four Seasons.'" &lt;em&gt;The Gazette Newspapers, &lt;/em&gt;May 4, 2011 by Jordan Edwards.&lt;/li&gt;
-&lt;li&gt;"Notes for a Haydn Anniversary." &lt;em&gt;Early Music America, &lt;/em&gt;Vol. 15, Winter 2008&lt;/li&gt;
-&lt;li&gt;"Modern Premiere: Biber." &lt;em&gt;Early Music America,&lt;/em&gt; Vol. 14, Fall 2008&lt;/li&gt;
-&lt;li&gt;"Religion That's Set to Music: The Bach Sinfonia. &lt;em&gt;The Washington Post Express, &lt;/em&gt;March 15, 2008 by Andrew Lindemann Malone&lt;/li&gt;
-&lt;li&gt;"Soundbytes: First complete performance in North America" [Bach, BWV 1127].&lt;span&gt; E&lt;/span&gt;&lt;em&gt;arly Music America,&lt;/em&gt; Vol. 11, Winter 2005. &lt;/li&gt;
-&lt;li&gt;Interviews with Judith Krummeck, WBJC Radio (Baltimore, Maryland) FM 90.9, regarding the upcoming premiere of Bach's rediscovered aria. Broadcasts: October 23-29, 2005 &lt;/li&gt;
-&lt;li&gt;Extended Interview and Discussion: FM Radio 95 (Cairo, Egypt) on T&lt;em&gt;own Beat; Cultural Activities Program&lt;/em&gt; (most important English language arts broadcast in the Middle East). Broadcast: May 2005&lt;/li&gt;
-&lt;li&gt;"Choral Concert . . ." &lt;em&gt;Akhbar El Nogoom&lt;/em&gt; [Leading artistic magazine in the Arabic world], May 7, 2005, p. 31 by Marianne Mahrous&lt;/li&gt;
-&lt;li&gt;"Fleur, The Obscure: Bach Sinfonia to Cast a Rare Light in the Overlooked Genre of Opera Comique." &lt;em&gt;The Washington Post, &lt;/em&gt;November 5, 2000 by Philip Kennicott.&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;&lt;div&gt;&lt;h3&gt;Exhibitions/Performances&lt;/h3&gt;&lt;p&gt;SELECTED PERFORMANCES&lt;/p&gt;
-&lt;p&gt;&lt;em&gt;Professional Conductor&lt;/em&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Conductor, Con el Coro Universidad and the Orquesta De Arcos, Teatro Santander Mayor, Bucaramanga, Colombia, May 2025&lt;/li&gt;
-&lt;li&gt;Conductor, World-Premiere: &lt;i&gt;Unity&lt;/i&gt;, Choral-Orchestral Commission, John Wineglass (composer), March 2025&lt;/li&gt;
-&lt;li&gt;Conductor, Antoník Dvořák Festival, Příbram, Czechia, May 2023&lt;/li&gt;
-&lt;li&gt;Conductor, Festival Bohuslav Matěj Čenohorský Music Festival, Nymburk, Slovakia, May 2023&lt;/li&gt;
-&lt;li&gt;Guest Conductor, Festival Hudba tisíců Máhler, Jihlava, Slovakia, May 22, 2023&lt;/li&gt;
-&lt;li&gt;Choral Preparation, Defiant Requiem Project 25&lt;sup&gt;th&lt;/sup&gt; Anniversary, Music Center at Strathmore/Concert Hall, April 2022&lt;/li&gt;
-&lt;li&gt;Conductor, First complete performance in mid-Atlantic region, &lt;i&gt;Considering Matthew Shepard&lt;/i&gt;, Washington, DC, 2019&lt;/li&gt;
-&lt;li&gt;Guest Conductor, Volos Municipal Conservatory Camerata, Volos, Greece, 2019&lt;/li&gt;
-&lt;li&gt;Guest Conductor, Ensemble Generabilis and Academia Athens Choir, Athens, Greece, 2019&lt;/li&gt;
-&lt;li&gt;Suducka Philharmonic Chamber Orchestra (Opole and Walbrzych, Poland, 2017)&lt;/li&gt;
-&lt;li&gt;Fryderyk Chopin University of Music Baroque Ensemble (Warsaw, Poland, 2017)&lt;/li&gt;
-&lt;li&gt;Re-Musica Festival of Contemporary Music (Prishtina, Kosovo, 2015)&lt;/li&gt;
-&lt;li&gt;Trinity Baroque Orchestra and Chorus (New York, 2014)&lt;/li&gt;
-&lt;li&gt;Governor of Vladimir Symphony Orchestra (Vladmir, Russian Federation, 2013)&lt;/li&gt;
-&lt;li&gt;Chamber Orchestra of the Orpheus Musical Theatre (Perm, Russian Federation, 2013)&lt;/li&gt;
-&lt;li&gt;B-A-C-H Chamber Orchestra (Yekaterinburg, Russian Federation, 2013)&lt;/li&gt;
-&lt;li&gt;Trinity Wall Street Chorus &amp;amp; Baroque Orchestra, October 2014&lt;/li&gt;
-&lt;li&gt;North American Premiere, Capel Bond: Concerto No. 1 for Trumpet &amp;amp; Strings
-&amp;amp; North American Premiere &amp;amp; Charles Avison: Concerto in B Major, Op. 6, No. 5, October 2012&lt;/li&gt;
-&lt;li&gt;First complete cycle (live performance) of Zelenka's Capriccios for Orchestra, May 2012&lt;/li&gt;
-&lt;li&gt;U.S. Premiere, Johann Bernhard Bach: Orchestral Suite No. 2, March 2011&lt;/li&gt;
-&lt;li&gt;Premiere of New Critical Edition, Antonio Salieri: Picciolo Requiem [premiere of new critical edition by Jane Schatkin Hettrick], October 2010&lt;/li&gt;
-&lt;li&gt;Henry Purcell: King Arthur, Concert Hall at The Arts Center at Strathmore, May 2009   &lt;/li&gt;
-&lt;li&gt;Modern premiere of Heinrich Ignaz Franz von Biber's Stabat Mater, May 2008&lt;/li&gt;
-&lt;li&gt;Concert before the Annual National Meeting of the American Musicological Society: Handel's Alexander's Feast and Johann Sebastian Bach: Alles mit Gott und nichts ohn’ ihn BWV 1127, October 2005 [before the Annual National Meeting of the American Musicological Society]&lt;/li&gt;
-&lt;li&gt;Washington area premiere: George Frideric Handel: Gloria, Washington, D.C., May 2002&lt;/li&gt;
-&lt;li&gt;Modern premiere: Marie-Emanuelle Bayon-Louis: Fleur d’Épine, before the International Conference Attending to Early Modern Women, November 2000&lt;/li&gt;
-&lt;li&gt;Programs with Tony Powell/Music &amp;amp; Movement, The John F. Kennedy Center for the Performing Arts, Washington, D.C., November 2000&lt;/li&gt;
-&lt;li&gt;Concert before the Annual National Meeting of the American Musicological Society: Cantata4, November 1996&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;em&gt;As Conductor at American University&lt;/em&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;American University Chamber Singers, nine international tours: 2025, 2023, 2019, 2017, 2015, 2013, 2011, 2009, 2006&lt;/li&gt;
-&lt;li&gt;Russian Federation Tour, American University Chamber Singers [Moscow (2 programs), Perm, Yekaterinburg (2 programs), Kazan]; programs with Governers Orchestra Vladimir, Chamber Orchestra of the Orpheus Theatre (Perm); B-A-C-H Chamber Orchestra (Yekaterinburg), May 2013&lt;/li&gt;
-&lt;li&gt;American University Chamber Singers, World Premiere, Fernando Benadon: Three Israeli Poems, September 2012&lt;/li&gt;
-&lt;li&gt;Spain &amp;amp; Portugal Tour, American&lt;/li&gt;
-&lt;li&gt;University Chamber Singers [Spain: Granada (2), Cordoba and Seville; Portugal: Faro and Lisbon (2)], May 2011   &lt;/li&gt;
-&lt;li&gt;U.S. Premiere, Juan Gutiérrez de Padilla: Missa Ero flos campi, American University Chamber Singers, April 2011&lt;/li&gt;
-&lt;li&gt;U.S. Premiere, Wilhem Friedemann Bach: Wohl dem, der den Herren fürchtet, Fk 76, American University Chamber Singers, November 2010&lt;/li&gt;
-&lt;li&gt;AU Chamber Singers International Tour of Hungary and Romania, May 2009&lt;/li&gt;
-&lt;li&gt;Invited Showcase Choir (AU Chamber Singers) for the Inaugural Washington, D.C. Choral Festival, Concert Hall, John F. Kennedy Center for the Performing Arts, May 2007&lt;/li&gt;
-&lt;li&gt;AU Chamber Singers Eastern United States and Eastern Canada Tour, October 2004&lt;/li&gt;
-&lt;li&gt;Various World Premieres&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;em&gt;Television &amp;amp; Radio Performances&lt;/em&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;Chorus Master, University Chorale, Christmas In Washington, National Television Broadcast: TNT, 2006-2008&lt;/li&gt;
-&lt;li&gt;Various performance broadcasts on National Public Radio's &lt;em&gt;Performance Today, Sunday Baroque, Great Sacred Music, &lt;/em&gt;and&lt;em&gt; Classical Discovies&lt;/em&gt;&lt;/li&gt;
-&lt;li&gt;Chorus Master, “A Tribute to Bill Cosby” for The Kennedy Center Honors Gala National Television Broadcast, PBS, 1999&lt;/li&gt;
-&lt;/ul&gt;
-&lt;p&gt;&lt;strong&gt;Reviews of Recent Live Performance&lt;/strong&gt;&lt;/p&gt;
-&lt;ul&gt;
-&lt;li&gt;“Concert Review: ‘Defiant Requiem: Verdi at Terezin’ at Strathmore Music Center.” &lt;i&gt;Maryland Theatre Guide&lt;/i&gt;, April 22, 2022 by Susan Brall.“At 20&lt;sup&gt;th&lt;/sup&gt; anniversary, ‘Defiant Requiem’ still makes a powerful statement.” &lt;i&gt;Washington Classical Review, &lt;/i&gt;April 21, 2022 by Andrew Lindemann Malone.&lt;/li&gt;
-&lt;li&gt;“Late Great Bach: The Mass in B Minor.” The Washington Post, October 27, 2014; critical review by Cecelia Porter.&lt;/li&gt;
-&lt;li&gt;“Bach Sinfonia’s Baroque Christmas Gifts.” The Washington Post, December 16, 2013, C4; critical review by Joan Reinthaler.&lt;/li&gt;
-&lt;li&gt;“The Sound of a Tradition.” MoCo Vox (The Voice of Montgomery County), December 16, 2013, critical review by David Cannon.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://dmvclassical.wordpress.com/2013/12/15/ill-be-baroque-for-christmas-bach-sinfonia/"&gt;“I’ll Be Baroque For Christmas: Bach Sinfonia at Montgomery College Cultural Arts Center.”&lt;/a&gt; DMV Classical, December 14, 2013; critical review by Andrew Lindemann Melone.&lt;/li&gt;
-&lt;li&gt;“Get Bach Loretta.” MoCo Vox (The Voice of Montgomery County), October 7, 2013, critical review by David Cannon.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://dmvclassical.wordpress.com/2013/10/06/the-trumpets-shall-sound-bach-sinfonia/"&gt;“The Trumpets Shall Sound: Bach Sinfonia at Montgomery College. Cultural Arts Center.”&lt;/a&gt; DMV Classical, October 7, 2013; critical review by Andrew Lindemann Melone.&lt;/li&gt;
-&lt;li&gt;“Хор хорош — «Камерные певцы Университета Америки» из Вашингтона выступили с концертом в Музее истории Екатеринбурга - Концерты - КультурМультур: ревиев” [“Good Choir — American University Chamber Singers from Washington gave a concert at the Museum of Yekaterinburg - Concerts - KulturMultur: Review.”] May 31, 2013.&lt;/li&gt;
-&lt;li&gt;“Bach Sinfonia rediscovers New World.” The Washington Post, May 8, 2013, teaser C1+C3; critical review by Cecelia Porter.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://dmvclassical.wordpress.com/2013/05/07/fiesta-bach-sinfonia-at-montgomery-colleges-cultural-arts-center/"&gt;“Fiesta! Bach Sinfonia at Montgomery College’s&lt;/a&gt; Cultural Arts Center in Silver Spring, May 5, 2013” DMV Classical, May 7, 2013; critical review by Andrew Lindemann Melone.&lt;/li&gt;
-&lt;li&gt; “Leipzig Idol: The Bach Sinfonia at Montgomery College’s Cultural Arts Center in Silver Spring.” DMV Classical, April 2, 2012; critical review by Andrew Lindemann Malone.&lt;/li&gt;
-&lt;li&gt;&lt;a href="https://www.washingtonpost.com/wp-dyn/content/article/2010/10/24/AR2010102402485.html"&gt;"Death becomes them: Mozart requiem and Bach Sinfonia."&lt;/a&gt; &lt;em&gt;The Washington Post, &lt;/em&gt;October 25, 2010; critical review by Cecelia Porter.  &lt;/li&gt;
-&lt;li&gt;&lt;a href="http://dmvclassical.wordpress.com/2010/03/08/mo-better-motets-the-bach-sinfonia-at-montgomery-college/;"&gt;Mo' Better Motets: The Bach Sinfonia and Sinfonia Voci.&lt;/a&gt; DMV Classical, March 8, 2010; critical review by Andrew Lindemann Malone.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://voices.washingtonpost.com/the-classical-beat/2010/03/in_performance_bach_sinfonia.html;"&gt;The Classical Beat: In Performance. Bach Sinfonia.&lt;/a&gt; &lt;em&gt;The Washington Post,&lt;/em&gt; March 8, 2010; critical review by Joan Reinthaler.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://www.washingtonpost.com/wp-dyn/content/article/2009/05/10/AR2009051002051.html;"&gt;Bach Sinfonia's 'King Arthur' at Strathmore Center.&lt;/a&gt;&lt;em&gt;The Washington Post, &lt;/em&gt;May 11, 2009; critical review by Cecelia Porter.&lt;/li&gt;
-&lt;li&gt;&lt;a href="http://www.washingtonpost.com/wp-dyn/content/article/2008/05/18/AR2008051802229.html;"&gt;Bach Sinfonia Workaday Wonders Of the Baroque.&lt;/a&gt;&lt;em&gt;The Washington Post,&lt;/em&gt; May 19, 2008; p. C01, critical review by Anne Midgette.&lt;/li&gt;
-&lt;li&gt;Music: The Bach Sinfonia. &lt;em&gt;The Washington Post, &lt;/em&gt;March 24, 2008; p. C05, critical review by Joan Reinthaler. &lt;/li&gt;
-&lt;li&gt;&lt;a href="http://www.washingtonpost.com/wp-dyn/content/article/2006/10/29/AR2006102900841.html;"&gt;Music: From Bach Sinfonia and Chantry, A Dido Die For.&lt;/a&gt; &lt;em&gt;The Washington Post,&lt;/em&gt; October 30, 2006; p. C05, critical review by Andrew Lindemann Malone. &lt;i&lt; li=""&gt; &lt;/i&lt;&gt;&lt;/li&gt;
-&lt;/ul&gt;
-&lt;/div&gt;
-&lt;/div&gt;
-</t>
+Anita Mannur is Director of the Asia, Pacific and Diaspora Studies and Professor of Critical Race,Gender, and Culture Studies. Her research areas are Asian American literature, food studies, transnational South Asia, fashion studies and race and gender studies. She is the author of two monograph, Culinary Fictions: Food in South Asian Diasporic Culture (Temple University Press, 2010) and Intimate Eating: Racialized Spaces and Radical Futures (Duke University Press 2022). She has co-edited several collections including Theorizing Diaspora (2005), Eating Asian America (2010) and Eating More Asian America (2025). Her work appears in several journals including American Quarterly, Cultural Studies, MELUS, Journal of Intercultural Studies, the Journal of Asian American Studies, Gastronomica, Amerasia Journal. She is the former editor-in-chief of the Journal of Asian American Studies and is a member of the editorial collective at Gastronomica: The Journal for Food Studies. &lt;br&gt;&lt;br/&gt;She was the 2012 recipient of the Early Career Award from the Association of Asian American Studies and the 2019 winner of the Excellence in Mentoring Award, also from the Association for Asian American Studies. She is President Elect of the Association for Asian American Studies.&lt;br/&gt;&lt;br/&gt;At AU, she teaches courses in Asian American Studies in South Asian popular culture, food and race and Asian American literature.&lt;br/&gt;&lt;br/&gt;In a former life, she was a certified spin instructor, but now she is happy to ride to the beat of the music as a student.
+&lt;/br&gt;</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>BA: University of Wisconsin Madison (Comparative Literature)&lt;br&gt;PhD: University of Massachusetts Amherst (Comparative Literature) &lt;p&gt;&lt;/p&gt;&lt;/br&gt;</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/migrated-profile-images/uploads/profiles/original/Anita_Mannur_046arw.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/content/dam/au/cf/profiles-migrated/am/amodel</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>profileCF</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>/conf/au/settings/dam/cfm/models/profiles</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>/content/dam/au/assets/global/images/au_profile.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>